<commit_message>
CORREÇÃO CENTRAL DE MODELOS
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/ORDEM_SERVICO_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/ORDEM_SERVICO_MODELO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7DD5E2-26CA-4EBB-8D59-9BAAA18960B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC5690-E2E1-4EBA-A7F5-2983AF37478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{90C1E774-E4E0-4641-BB0D-47F1E26D8AAD}"/>
   </bookViews>
@@ -235,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -450,9 +456,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -462,143 +585,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,7 +927,7 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:F31"/>
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,44 +956,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
     </row>
     <row r="2" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="17"/>
       <c r="H2" s="15" t="s">
         <v>11</v>
@@ -1029,15 +1038,15 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="15"/>
       <c r="K3" s="14">
         <v>1</v>
@@ -1073,9 +1082,9 @@
         <v>9</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="15"/>
       <c r="K4" s="14">
         <v>2</v>
@@ -1102,16 +1111,16 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="15"/>
       <c r="K5" s="14">
         <v>3</v>
@@ -1138,16 +1147,16 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="53" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="15"/>
       <c r="K6" s="14">
         <v>4</v>
@@ -1171,17 +1180,17 @@
       <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="15"/>
       <c r="K7" s="14">
         <v>5</v>
@@ -1205,17 +1214,17 @@
       <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="53" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="15"/>
       <c r="K8" s="14">
         <v>6</v>
@@ -1249,9 +1258,9 @@
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="15"/>
       <c r="K9" s="14">
         <v>7</v>
@@ -1278,425 +1287,425 @@
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
+      <c r="U11" s="55"/>
+      <c r="V11" s="55"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
+      <c r="B12" s="50"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="25" t="s">
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="30"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="23"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="20" t="s">
+      <c r="K13" s="52"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="33"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="64"/>
+      <c r="U13" s="64"/>
+      <c r="V13" s="65"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="33"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="64"/>
+      <c r="U14" s="64"/>
+      <c r="V14" s="65"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="45"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="20" t="s">
+      <c r="K15" s="52"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="33"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="64"/>
+      <c r="U15" s="64"/>
+      <c r="V15" s="65"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
+      <c r="B16" s="49"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="36"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="43"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="25" t="s">
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="30"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="23"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="H18" s="40" t="s">
+      <c r="B18" s="49"/>
+      <c r="H18" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="40"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="20" t="s">
+      <c r="K18" s="52"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="33"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="64"/>
+      <c r="U18" s="64"/>
+      <c r="V18" s="65"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="33"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="64"/>
+      <c r="U19" s="64"/>
+      <c r="V19" s="65"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="42"/>
+      <c r="B20" s="49"/>
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
       <c r="I20" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J20" s="15"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="20" t="s">
+      <c r="K20" s="52"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="33"/>
+      <c r="Q20" s="60"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="64"/>
+      <c r="U20" s="64"/>
+      <c r="V20" s="65"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
       <c r="H21" s="11"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="36"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="61"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="43"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="49"/>
       <c r="G22" s="11"/>
       <c r="H22" s="12"/>
       <c r="I22" s="10" t="s">
         <v>25</v>
       </c>
       <c r="J22" s="15"/>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="25" t="s">
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="30"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="23"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="20" t="s">
+      <c r="K23" s="52"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="33"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="61"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="64"/>
+      <c r="V23" s="65"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="49"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="33"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="64"/>
+      <c r="V24" s="65"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="20" t="s">
+      <c r="K25" s="52"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="32"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="33"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="64"/>
+      <c r="U25" s="64"/>
+      <c r="V25" s="65"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J26" s="15"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="36"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="43"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -1710,37 +1719,37 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="37" t="s">
+      <c r="K28" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="37"/>
-      <c r="V28" s="37"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
     </row>
     <row r="29" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="A29" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19" t="s">
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="29" t="s">
+      <c r="F29" s="37"/>
+      <c r="G29" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
       <c r="J29" s="15"/>
       <c r="K29" s="13" t="s">
         <v>28</v>
@@ -1780,12 +1789,12 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="62"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
       <c r="G30" s="17"/>
       <c r="H30" s="15" t="s">
         <v>11</v>
@@ -1814,15 +1823,15 @@
       <c r="V30" s="14"/>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
       <c r="J31" s="15"/>
       <c r="K31" s="14">
         <v>2</v>
@@ -1858,9 +1867,9 @@
         <v>9</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="49"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
       <c r="J32" s="15"/>
       <c r="K32" s="14">
         <v>3</v>
@@ -1887,16 +1896,16 @@
       <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="52"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
       <c r="J33" s="15"/>
       <c r="K33" s="14">
         <v>4</v>
@@ -1923,16 +1932,16 @@
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="53" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="15"/>
       <c r="K34" s="14">
         <v>5</v>
@@ -1956,17 +1965,17 @@
       <c r="V34" s="14"/>
     </row>
     <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
       <c r="J35" s="15"/>
       <c r="K35" s="14">
         <v>6</v>
@@ -1990,17 +1999,17 @@
       <c r="V35" s="14"/>
     </row>
     <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="53" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
       <c r="J36" s="15"/>
       <c r="K36" s="14">
         <v>7</v>
@@ -2034,438 +2043,499 @@
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="45"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="25"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="38" t="s">
+      <c r="K37" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="38"/>
-      <c r="V37" s="38"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="54"/>
+      <c r="T37" s="54"/>
+      <c r="U37" s="54"/>
+      <c r="V37" s="54"/>
     </row>
     <row r="38" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="45"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="25"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="39" t="s">
+      <c r="K38" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="39"/>
-      <c r="S38" s="39"/>
-      <c r="T38" s="39"/>
-      <c r="U38" s="39"/>
-      <c r="V38" s="39"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="55"/>
+      <c r="P38" s="55"/>
+      <c r="Q38" s="55"/>
+      <c r="R38" s="55"/>
+      <c r="S38" s="55"/>
+      <c r="T38" s="55"/>
+      <c r="U38" s="55"/>
+      <c r="V38" s="55"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="45"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="25"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="23" t="s">
+      <c r="K39" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="24"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="25" t="s">
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q39" s="26"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="29"/>
-      <c r="U39" s="29"/>
-      <c r="V39" s="30"/>
+      <c r="Q39" s="57"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="62"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="23"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="45"/>
+      <c r="B40" s="50"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="20" t="s">
+      <c r="K40" s="52"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="67"/>
+      <c r="P40" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="31"/>
-      <c r="T40" s="32"/>
-      <c r="U40" s="32"/>
-      <c r="V40" s="33"/>
+      <c r="Q40" s="60"/>
+      <c r="R40" s="61"/>
+      <c r="S40" s="63"/>
+      <c r="T40" s="64"/>
+      <c r="U40" s="64"/>
+      <c r="V40" s="65"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="45"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="25"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="31"/>
-      <c r="T41" s="32"/>
-      <c r="U41" s="32"/>
-      <c r="V41" s="33"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="67"/>
+      <c r="N41" s="67"/>
+      <c r="O41" s="67"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="61"/>
+      <c r="S41" s="63"/>
+      <c r="T41" s="64"/>
+      <c r="U41" s="64"/>
+      <c r="V41" s="65"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="45"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="25"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="20" t="s">
+      <c r="K42" s="52"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="32"/>
-      <c r="U42" s="32"/>
-      <c r="V42" s="33"/>
+      <c r="Q42" s="60"/>
+      <c r="R42" s="61"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="64"/>
+      <c r="U42" s="64"/>
+      <c r="V42" s="65"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="45"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="25"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="24"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="21"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="34"/>
-      <c r="T43" s="35"/>
-      <c r="U43" s="35"/>
-      <c r="V43" s="36"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="67"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="60"/>
+      <c r="R43" s="61"/>
+      <c r="S43" s="66"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="42"/>
+      <c r="V43" s="43"/>
     </row>
     <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="42"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="45"/>
+      <c r="B44" s="49"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="25"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="23" t="s">
+      <c r="K44" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="24"/>
-      <c r="P44" s="25" t="s">
+      <c r="L44" s="67"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="67"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q44" s="26"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="28"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="30"/>
+      <c r="Q44" s="57"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+      <c r="V44" s="23"/>
     </row>
     <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="20" t="s">
+      <c r="K45" s="52"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
+      <c r="P45" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q45" s="21"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="31"/>
-      <c r="T45" s="32"/>
-      <c r="U45" s="32"/>
-      <c r="V45" s="33"/>
+      <c r="Q45" s="60"/>
+      <c r="R45" s="61"/>
+      <c r="S45" s="63"/>
+      <c r="T45" s="64"/>
+      <c r="U45" s="64"/>
+      <c r="V45" s="65"/>
     </row>
     <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="42"/>
-      <c r="H46" s="40" t="s">
+      <c r="B46" s="49"/>
+      <c r="H46" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I46" s="40"/>
+      <c r="I46" s="53"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="21"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="31"/>
-      <c r="T46" s="32"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="33"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
+      <c r="O46" s="67"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="60"/>
+      <c r="R46" s="61"/>
+      <c r="S46" s="63"/>
+      <c r="T46" s="64"/>
+      <c r="U46" s="64"/>
+      <c r="V46" s="65"/>
     </row>
     <row r="47" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="20" t="s">
+      <c r="K47" s="52"/>
+      <c r="L47" s="67"/>
+      <c r="M47" s="67"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="22"/>
-      <c r="S47" s="31"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="33"/>
+      <c r="Q47" s="60"/>
+      <c r="R47" s="61"/>
+      <c r="S47" s="63"/>
+      <c r="T47" s="64"/>
+      <c r="U47" s="64"/>
+      <c r="V47" s="65"/>
     </row>
     <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="42"/>
+      <c r="B48" s="49"/>
       <c r="G48" s="11"/>
       <c r="H48" s="12"/>
       <c r="I48" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J48" s="15"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="20"/>
-      <c r="Q48" s="21"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="35"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="36"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="67"/>
+      <c r="M48" s="67"/>
+      <c r="N48" s="67"/>
+      <c r="O48" s="67"/>
+      <c r="P48" s="59"/>
+      <c r="Q48" s="60"/>
+      <c r="R48" s="61"/>
+      <c r="S48" s="66"/>
+      <c r="T48" s="42"/>
+      <c r="U48" s="42"/>
+      <c r="V48" s="43"/>
     </row>
     <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="23" t="s">
+      <c r="K49" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="25" t="s">
+      <c r="L49" s="67"/>
+      <c r="M49" s="67"/>
+      <c r="N49" s="67"/>
+      <c r="O49" s="67"/>
+      <c r="P49" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="Q49" s="26"/>
-      <c r="R49" s="27"/>
-      <c r="S49" s="28"/>
-      <c r="T49" s="29"/>
-      <c r="U49" s="29"/>
-      <c r="V49" s="30"/>
+      <c r="Q49" s="57"/>
+      <c r="R49" s="58"/>
+      <c r="S49" s="62"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+      <c r="V49" s="23"/>
     </row>
     <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="42"/>
+      <c r="B50" s="49"/>
       <c r="G50" s="11"/>
       <c r="H50" s="12"/>
       <c r="I50" s="10" t="s">
         <v>25</v>
       </c>
       <c r="J50" s="15"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="20" t="s">
+      <c r="K50" s="52"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="67"/>
+      <c r="N50" s="67"/>
+      <c r="O50" s="67"/>
+      <c r="P50" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="32"/>
-      <c r="U50" s="32"/>
-      <c r="V50" s="33"/>
+      <c r="Q50" s="60"/>
+      <c r="R50" s="61"/>
+      <c r="S50" s="63"/>
+      <c r="T50" s="64"/>
+      <c r="U50" s="64"/>
+      <c r="V50" s="65"/>
     </row>
     <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="31"/>
-      <c r="T51" s="32"/>
-      <c r="U51" s="32"/>
-      <c r="V51" s="33"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="67"/>
+      <c r="M51" s="67"/>
+      <c r="N51" s="67"/>
+      <c r="O51" s="67"/>
+      <c r="P51" s="59"/>
+      <c r="Q51" s="60"/>
+      <c r="R51" s="61"/>
+      <c r="S51" s="63"/>
+      <c r="T51" s="64"/>
+      <c r="U51" s="64"/>
+      <c r="V51" s="65"/>
     </row>
     <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="42"/>
+      <c r="B52" s="49"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="20" t="s">
+      <c r="K52" s="52"/>
+      <c r="L52" s="67"/>
+      <c r="M52" s="67"/>
+      <c r="N52" s="67"/>
+      <c r="O52" s="67"/>
+      <c r="P52" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q52" s="21"/>
-      <c r="R52" s="22"/>
-      <c r="S52" s="31"/>
-      <c r="T52" s="32"/>
-      <c r="U52" s="32"/>
-      <c r="V52" s="33"/>
+      <c r="Q52" s="60"/>
+      <c r="R52" s="61"/>
+      <c r="S52" s="63"/>
+      <c r="T52" s="64"/>
+      <c r="U52" s="64"/>
+      <c r="V52" s="65"/>
     </row>
     <row r="53" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
       <c r="J53" s="15"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="34"/>
-      <c r="T53" s="35"/>
-      <c r="U53" s="35"/>
-      <c r="V53" s="36"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="67"/>
+      <c r="N53" s="67"/>
+      <c r="O53" s="67"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="60"/>
+      <c r="R53" s="61"/>
+      <c r="S53" s="66"/>
+      <c r="T53" s="42"/>
+      <c r="U53" s="42"/>
+      <c r="V53" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="P45:R46"/>
+    <mergeCell ref="P47:R48"/>
+    <mergeCell ref="K49:K53"/>
+    <mergeCell ref="L49:O53"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="S49:V53"/>
+    <mergeCell ref="P50:R51"/>
+    <mergeCell ref="P52:R53"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A41:F42"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="K28:V28"/>
+    <mergeCell ref="K37:V37"/>
+    <mergeCell ref="K39:K43"/>
+    <mergeCell ref="L39:O43"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="S39:V43"/>
+    <mergeCell ref="P40:R41"/>
+    <mergeCell ref="P42:R43"/>
+    <mergeCell ref="K44:K48"/>
+    <mergeCell ref="L44:O48"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="S44:V48"/>
+    <mergeCell ref="K38:V38"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="P20:R21"/>
+    <mergeCell ref="P23:R24"/>
+    <mergeCell ref="P25:R26"/>
+    <mergeCell ref="S12:V16"/>
+    <mergeCell ref="S17:V21"/>
+    <mergeCell ref="S22:V26"/>
+    <mergeCell ref="K22:K26"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P13:R14"/>
+    <mergeCell ref="P15:R16"/>
+    <mergeCell ref="L12:O16"/>
+    <mergeCell ref="L17:O21"/>
+    <mergeCell ref="L22:O26"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K17:K21"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K10:V10"/>
+    <mergeCell ref="K11:V11"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G32:I33"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:F36"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
     <mergeCell ref="A29:D31"/>
     <mergeCell ref="G29:I29"/>
     <mergeCell ref="H31:I31"/>
@@ -2490,83 +2560,22 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:F14"/>
-    <mergeCell ref="K1:V1"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="K17:K21"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="K10:V10"/>
-    <mergeCell ref="K11:V11"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G32:I33"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:F36"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="P20:R21"/>
-    <mergeCell ref="P23:R24"/>
-    <mergeCell ref="P25:R26"/>
-    <mergeCell ref="S12:V16"/>
-    <mergeCell ref="S17:V21"/>
-    <mergeCell ref="S22:V26"/>
-    <mergeCell ref="K22:K26"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P13:R14"/>
-    <mergeCell ref="P15:R16"/>
-    <mergeCell ref="L12:O16"/>
-    <mergeCell ref="L17:O21"/>
-    <mergeCell ref="L22:O26"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="K28:V28"/>
-    <mergeCell ref="K37:V37"/>
-    <mergeCell ref="K39:K43"/>
-    <mergeCell ref="L39:O43"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="S39:V43"/>
-    <mergeCell ref="P40:R41"/>
-    <mergeCell ref="P42:R43"/>
-    <mergeCell ref="K44:K48"/>
-    <mergeCell ref="L44:O48"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="S44:V48"/>
-    <mergeCell ref="K38:V38"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="P45:R46"/>
-    <mergeCell ref="P47:R48"/>
-    <mergeCell ref="K49:K53"/>
-    <mergeCell ref="L49:O53"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="S49:V53"/>
-    <mergeCell ref="P50:R51"/>
-    <mergeCell ref="P52:R53"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A41:F42"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>

</xml_diff>